<commit_message>
added dining and grocery bbn
</commit_message>
<xml_diff>
--- a/Input Files/Micropolis_pop_at_node.xlsx
+++ b/Input Files/Micropolis_pop_at_node.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oitncsu-my.sharepoint.com/personal/bvizank_ncsu_edu/Documents/Research/src/ABM/Main_code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squar\Documents\hydraulic_ABM\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{86DD1F1E-B2BC-4412-A021-242B7666A2F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F29A1AF2-8C48-478C-BF3F-3326671948C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87206080-8D89-444F-8155-8E883D8BA887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="2715" windowWidth="24240" windowHeight="13140" xr2:uid="{776854DF-CE84-3D47-9E0F-6A96FE1D0219}"/>
+    <workbookView xWindow="25860" yWindow="-960" windowWidth="21600" windowHeight="11385" xr2:uid="{776854DF-CE84-3D47-9E0F-6A96FE1D0219}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="688">
   <si>
     <t>Max Population</t>
   </si>
@@ -2095,6 +2095,9 @@
   </si>
   <si>
     <t>Node</t>
+  </si>
+  <si>
+    <t>Commercial</t>
   </si>
 </sst>
 </file>
@@ -2115,12 +2118,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2136,10 +2151,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2457,15 +2476,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF96AF72-2F4F-8647-B8E7-58F73E65F459}">
   <dimension ref="A1:M687"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G254" sqref="G254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.125" customWidth="1"/>
     <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2487,6 +2506,9 @@
       <c r="B2" s="1">
         <v>30</v>
       </c>
+      <c r="D2" s="4" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -4633,18 +4655,18 @@
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="1" t="s">
+      <c r="A271" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="B271" s="1">
+      <c r="B271" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="1" t="s">
+      <c r="A272" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B272" s="1">
+      <c r="B272" s="3">
         <v>275</v>
       </c>
     </row>
@@ -4769,18 +4791,18 @@
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="1" t="s">
+      <c r="A288" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="B288" s="1">
+      <c r="B288" s="5">
         <v>80</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="1" t="s">
+      <c r="A289" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B289" s="1">
+      <c r="B289" s="6">
         <v>36</v>
       </c>
     </row>
@@ -4817,10 +4839,10 @@
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="1" t="s">
+      <c r="A294" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B294" s="1">
+      <c r="B294" s="3">
         <v>700</v>
       </c>
     </row>
@@ -4849,42 +4871,42 @@
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="1" t="s">
+      <c r="A298" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B298" s="1">
+      <c r="B298" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" s="1" t="s">
+      <c r="A299" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B299" s="1">
+      <c r="B299" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" s="1" t="s">
+      <c r="A300" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B300" s="1">
+      <c r="B300" s="3">
         <v>46</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" s="1" t="s">
+      <c r="A301" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B301" s="1">
+      <c r="B301" s="3">
         <v>50</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A302" s="1" t="s">
+      <c r="A302" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="B302" s="1">
+      <c r="B302" s="3">
         <v>20</v>
       </c>
     </row>
@@ -5601,18 +5623,18 @@
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A392" s="1" t="s">
+      <c r="A392" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="B392" s="1">
+      <c r="B392" s="3">
         <v>500</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A393" s="1" t="s">
+      <c r="A393" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="B393" s="1">
+      <c r="B393" s="3">
         <v>375</v>
       </c>
     </row>
@@ -6145,34 +6167,34 @@
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A460" s="1" t="s">
+      <c r="A460" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B460" s="1">
+      <c r="B460" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A461" s="1" t="s">
+      <c r="A461" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="B461" s="1">
+      <c r="B461" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A462" s="1" t="s">
+      <c r="A462" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="B462" s="1">
+      <c r="B462" s="3">
         <v>10</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A463" s="1" t="s">
+      <c r="A463" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="B463" s="1">
+      <c r="B463" s="6">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nearly done with movement
</commit_message>
<xml_diff>
--- a/Input Files/Micropolis_pop_at_node.xlsx
+++ b/Input Files/Micropolis_pop_at_node.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\squar\Documents\hydraulic_ABM\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87206080-8D89-444F-8155-8E883D8BA887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976EAF0A-333F-4CBE-BCCA-62C638586D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25860" yWindow="-960" windowWidth="21600" windowHeight="11385" xr2:uid="{776854DF-CE84-3D47-9E0F-6A96FE1D0219}"/>
+    <workbookView xWindow="-22965" yWindow="4350" windowWidth="21600" windowHeight="11385" xr2:uid="{776854DF-CE84-3D47-9E0F-6A96FE1D0219}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2476,8 +2476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF96AF72-2F4F-8647-B8E7-58F73E65F459}">
   <dimension ref="A1:M687"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G254" sqref="G254"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>